<commit_message>
add scripts and results of eaglerc ngi mode
</commit_message>
<xml_diff>
--- a/files/SI_Data_1__CS_tagRNASeq.xlsx
+++ b/files/SI_Data_1__CS_tagRNASeq.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsun/Google Drive/projects/HuoberBrezel/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonk414/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179C7162-AD75-8D49-9F09-6E1220E24084}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7768661A-844C-C145-A744-5D0CAF99D36D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24760" windowHeight="15440" activeTab="4" xr2:uid="{0A1B866E-BAB2-5B48-9BA1-056163FF4A88}"/>
+    <workbookView xWindow="6720" yWindow="1120" windowWidth="18420" windowHeight="15440" activeTab="2" xr2:uid="{0A1B866E-BAB2-5B48-9BA1-056163FF4A88}"/>
   </bookViews>
   <sheets>
     <sheet name="Trimmomatic" sheetId="2" r:id="rId1"/>
     <sheet name="HISAT2" sheetId="1" r:id="rId2"/>
     <sheet name="STAR" sheetId="4" r:id="rId3"/>
     <sheet name="EAGLE-RC" sheetId="3" r:id="rId4"/>
-    <sheet name="Overlap" sheetId="5" r:id="rId5"/>
+    <sheet name="EAGLE-RC (ngi)" sheetId="6" r:id="rId5"/>
+    <sheet name="Overlap" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="59">
   <si>
     <t>library name</t>
   </si>
@@ -175,9 +176,6 @@
   </si>
   <si>
     <t>EAGLE-RC step</t>
-  </si>
-  <si>
-    <t>N + O + P</t>
   </si>
   <si>
     <t>* I: this may contains reads that were mapped on ChrUn</t>
@@ -350,7 +348,7 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -419,13 +417,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -1017,7 +1016,7 @@
         <v>38</v>
       </c>
       <c r="S1" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -1551,7 +1550,7 @@
         <v>42</v>
       </c>
       <c r="I10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S10" t="s">
         <v>41</v>
@@ -1570,7 +1569,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="M13" s="46">
-        <f t="shared" ref="M13:M19" si="13">SUM(J3:L3)</f>
+        <f t="shared" ref="M13:M17" si="13">SUM(J3:L3)</f>
         <v>729386</v>
       </c>
     </row>
@@ -1619,8 +1618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4A77191-EB84-9140-9493-17DED251511A}">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1691,7 +1690,7 @@
         <v>38</v>
       </c>
       <c r="S1" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -1747,15 +1746,15 @@
         <v>0.33367080733771076</v>
       </c>
       <c r="P2">
-        <v>196.32499999999999</v>
+        <v>77.837000000000003</v>
       </c>
       <c r="Q2" s="27">
         <f t="shared" ref="Q2:Q7" si="1">P2/D2*1000000</f>
-        <v>95.673132918039073</v>
+        <v>37.931540287489668</v>
       </c>
       <c r="R2" s="27">
         <f>Q2/60</f>
-        <v>1.5945522153006513</v>
+        <v>0.63219233812482778</v>
       </c>
       <c r="S2" s="3">
         <f t="shared" ref="S2:S7" si="2">(J2+K2+L2)/D2</f>
@@ -1815,15 +1814,15 @@
         <v>0.33413366709697712</v>
       </c>
       <c r="P3">
-        <v>199.75399999999999</v>
+        <v>74.204999999999998</v>
       </c>
       <c r="Q3" s="27">
         <f t="shared" si="1"/>
-        <v>163.00288135994313</v>
+        <v>60.552623783827009</v>
       </c>
       <c r="R3" s="27">
         <f>Q3/60</f>
-        <v>2.7167146893323855</v>
+        <v>1.0092103963971168</v>
       </c>
       <c r="S3" s="3">
         <f t="shared" si="2"/>
@@ -1883,15 +1882,15 @@
         <v>0.33179988978250496</v>
       </c>
       <c r="P4">
-        <v>204.89400000000001</v>
+        <v>220.416</v>
       </c>
       <c r="Q4" s="27">
         <f t="shared" si="1"/>
-        <v>72.136503583166245</v>
+        <v>77.601294199865151</v>
       </c>
       <c r="R4" s="27">
         <f t="shared" ref="R4:R6" si="6">Q4/60</f>
-        <v>1.2022750597194374</v>
+        <v>1.2933549033310858</v>
       </c>
       <c r="S4" s="3">
         <f t="shared" si="2"/>
@@ -1951,15 +1950,15 @@
         <v>0.33385114278654782</v>
       </c>
       <c r="P5">
-        <v>80.781999999999996</v>
+        <v>79.706999999999994</v>
       </c>
       <c r="Q5" s="27">
         <f t="shared" si="1"/>
-        <v>58.768624820581159</v>
+        <v>57.98656604904636</v>
       </c>
       <c r="R5" s="27">
         <f t="shared" si="6"/>
-        <v>0.97947708034301928</v>
+        <v>0.96644276748410596</v>
       </c>
       <c r="S5" s="3">
         <f t="shared" si="2"/>
@@ -2019,15 +2018,15 @@
         <v>0.33025897081260164</v>
       </c>
       <c r="P6">
-        <v>84.796999999999997</v>
+        <v>87.731999999999999</v>
       </c>
       <c r="Q6" s="27">
         <f t="shared" si="1"/>
-        <v>25.380785108135548</v>
+        <v>26.259266708809839</v>
       </c>
       <c r="R6" s="27">
         <f t="shared" si="6"/>
-        <v>0.42301308513559249</v>
+        <v>0.43765444514683066</v>
       </c>
       <c r="S6" s="3">
         <f t="shared" si="2"/>
@@ -2087,15 +2086,15 @@
         <v>0.33560827015376704</v>
       </c>
       <c r="P7">
-        <v>218.333</v>
+        <v>86.058000000000007</v>
       </c>
       <c r="Q7" s="27">
         <f t="shared" si="1"/>
-        <v>68.741530610702796</v>
+        <v>27.095119112987323</v>
       </c>
       <c r="R7" s="27">
         <f>Q7/60</f>
-        <v>1.1456921768450465</v>
+        <v>0.45158531854978873</v>
       </c>
       <c r="S7" s="3">
         <f t="shared" si="2"/>
@@ -2146,15 +2145,15 @@
       </c>
       <c r="P8" s="21">
         <f t="shared" si="7"/>
-        <v>164.14750000000001</v>
+        <v>104.32583333333332</v>
       </c>
       <c r="Q8" s="21">
         <f t="shared" si="7"/>
-        <v>80.617243066761333</v>
+        <v>47.904401690337558</v>
       </c>
       <c r="R8" s="21">
         <f t="shared" si="7"/>
-        <v>1.3436207177793555</v>
+        <v>0.79840669483895921</v>
       </c>
       <c r="S8" s="17">
         <f t="shared" si="7"/>
@@ -2205,15 +2204,15 @@
       </c>
       <c r="P9" s="22">
         <f t="shared" si="8"/>
-        <v>63.475772482893042</v>
+        <v>57.098171043971888</v>
       </c>
       <c r="Q9" s="22">
         <f t="shared" si="8"/>
-        <v>46.379860094223503</v>
+        <v>20.710041329353579</v>
       </c>
       <c r="R9" s="22">
         <f t="shared" si="8"/>
-        <v>0.77299766823705851</v>
+        <v>0.34516735548922656</v>
       </c>
       <c r="S9" s="13">
         <f t="shared" si="8"/>
@@ -2225,7 +2224,7 @@
         <v>42</v>
       </c>
       <c r="I10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S10" t="s">
         <v>41</v>
@@ -2238,10 +2237,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004FEFD4-A36D-7843-8AFA-92A18F957172}">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2252,12 +2251,12 @@
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="12" width="16.1640625" customWidth="1"/>
     <col min="13" max="15" width="11.6640625" customWidth="1"/>
-    <col min="16" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -2298,31 +2297,28 @@
         <v>35</v>
       </c>
       <c r="N1" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="45" t="s">
+      <c r="P1" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="45" t="s">
+      <c r="Q1" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="R1" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="T1" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="U1" s="24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>13</v>
       </c>
@@ -2374,28 +2370,24 @@
       <c r="P2" s="4">
         <v>90576</v>
       </c>
-      <c r="Q2" s="4">
-        <f>SUM(N2:P2)</f>
-        <v>283053</v>
+      <c r="Q2" s="3">
+        <f>N2/(N2+O2+P2)</f>
+        <v>0.32739098331407901</v>
       </c>
       <c r="R2" s="3">
-        <f>N2/Q2</f>
-        <v>0.32739098331407901</v>
+        <f>O2/(N2+O2+P2)</f>
+        <v>0.35261240827689516</v>
       </c>
       <c r="S2" s="3">
-        <f>O2/Q2</f>
-        <v>0.35261240827689516</v>
+        <f>P2/(N2+O2+P2)</f>
+        <v>0.31999660840902588</v>
       </c>
       <c r="T2" s="3">
-        <f>P2/Q2</f>
-        <v>0.31999660840902588</v>
-      </c>
-      <c r="U2" s="3">
-        <f t="shared" ref="U2:U7" si="0">Q2/D2</f>
+        <f>(N2+O2+P2)/D2</f>
         <v>0.13616107292152721</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -2415,7 +2407,7 @@
         <v>267473</v>
       </c>
       <c r="G3" s="30">
-        <f t="shared" ref="G3:G7" si="1">D3-E3-F3</f>
+        <f t="shared" ref="G3:G7" si="0">D3-E3-F3</f>
         <v>233072</v>
       </c>
       <c r="H3">
@@ -2425,7 +2417,7 @@
         <v>232553</v>
       </c>
       <c r="J3" s="4">
-        <f t="shared" ref="J3:J7" si="2">D3-H3-I3</f>
+        <f t="shared" ref="J3:J7" si="1">D3-H3-I3</f>
         <v>225957</v>
       </c>
       <c r="K3" s="32">
@@ -2435,7 +2427,7 @@
         <v>264296</v>
       </c>
       <c r="M3" s="30">
-        <f t="shared" ref="M3:M7" si="3">D3-K3-L3</f>
+        <f t="shared" ref="M3:M7" si="2">D3-K3-L3</f>
         <v>214509</v>
       </c>
       <c r="N3" s="4">
@@ -2447,28 +2439,24 @@
       <c r="P3" s="4">
         <v>58708</v>
       </c>
-      <c r="Q3" s="4">
-        <f t="shared" ref="Q3:Q7" si="4">SUM(N3:P3)</f>
-        <v>181968</v>
+      <c r="Q3" s="3">
+        <f t="shared" ref="Q3:Q7" si="3">N3/(N3+O3+P3)</f>
+        <v>0.31875934230194319</v>
       </c>
       <c r="R3" s="3">
-        <f t="shared" ref="R3:R7" si="5">N3/Q3</f>
-        <v>0.31875934230194319</v>
+        <f t="shared" ref="R3:R7" si="4">O3/(N3+O3+P3)</f>
+        <v>0.35861250329728306</v>
       </c>
       <c r="S3" s="3">
-        <f t="shared" ref="S3:S7" si="6">O3/Q3</f>
-        <v>0.35861250329728306</v>
+        <f t="shared" ref="S3:S7" si="5">P3/(N3+O3+P3)</f>
+        <v>0.32262815440077375</v>
       </c>
       <c r="T3" s="3">
-        <f t="shared" ref="T3:T7" si="7">P3/Q3</f>
-        <v>0.32262815440077375</v>
-      </c>
-      <c r="U3" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="T3:T7" si="6">(N3+O3+P3)/D3</f>
         <v>0.14659564389362051</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -2488,7 +2476,7 @@
         <v>688541</v>
       </c>
       <c r="G4" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>510812</v>
       </c>
       <c r="H4">
@@ -2498,7 +2486,7 @@
         <v>573611</v>
       </c>
       <c r="J4" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>497086</v>
       </c>
       <c r="K4" s="32">
@@ -2508,7 +2496,7 @@
         <v>674657</v>
       </c>
       <c r="M4" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>466563</v>
       </c>
       <c r="N4" s="4">
@@ -2520,28 +2508,24 @@
       <c r="P4" s="4">
         <v>135468</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="3">
+        <f t="shared" si="3"/>
+        <v>0.32063417710951775</v>
+      </c>
+      <c r="R4" s="3">
         <f t="shared" si="4"/>
-        <v>431236</v>
-      </c>
-      <c r="R4" s="3">
+        <v>0.36522692910610433</v>
+      </c>
+      <c r="S4" s="3">
         <f t="shared" si="5"/>
-        <v>0.32063417710951775</v>
-      </c>
-      <c r="S4" s="3">
+        <v>0.31413889378437793</v>
+      </c>
+      <c r="T4" s="3">
         <f t="shared" si="6"/>
-        <v>0.36522692910610433</v>
-      </c>
-      <c r="T4" s="3">
-        <f t="shared" si="7"/>
-        <v>0.31413889378437793</v>
-      </c>
-      <c r="U4" s="3">
-        <f t="shared" si="0"/>
         <v>0.15004397953559837</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -2561,7 +2545,7 @@
         <v>316903</v>
       </c>
       <c r="G5" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>281770</v>
       </c>
       <c r="H5">
@@ -2571,7 +2555,7 @@
         <v>306821</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>264228</v>
       </c>
       <c r="K5" s="32">
@@ -2581,7 +2565,7 @@
         <v>319842</v>
       </c>
       <c r="M5" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>253415</v>
       </c>
       <c r="N5" s="4">
@@ -2593,28 +2577,24 @@
       <c r="P5" s="4">
         <v>58625</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="3">
+        <f t="shared" si="3"/>
+        <v>0.33573796169140235</v>
+      </c>
+      <c r="R5" s="3">
         <f t="shared" si="4"/>
-        <v>181317</v>
-      </c>
-      <c r="R5" s="3">
+        <v>0.34093328259346889</v>
+      </c>
+      <c r="S5" s="3">
         <f t="shared" si="5"/>
-        <v>0.33573796169140235</v>
-      </c>
-      <c r="S5" s="3">
+        <v>0.32332875571512876</v>
+      </c>
+      <c r="T5" s="3">
         <f t="shared" si="6"/>
-        <v>0.34093328259346889</v>
-      </c>
-      <c r="T5" s="3">
-        <f t="shared" si="7"/>
-        <v>0.32332875571512876</v>
-      </c>
-      <c r="U5" s="3">
-        <f t="shared" si="0"/>
         <v>0.13015211942149829</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
@@ -2634,7 +2614,7 @@
         <v>697859</v>
       </c>
       <c r="G6" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>650497</v>
       </c>
       <c r="H6">
@@ -2644,7 +2624,7 @@
         <v>627022</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>622650</v>
       </c>
       <c r="K6" s="32">
@@ -2654,7 +2634,7 @@
         <v>696599</v>
       </c>
       <c r="M6" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>593919</v>
       </c>
       <c r="N6" s="4">
@@ -2666,28 +2646,24 @@
       <c r="P6" s="4">
         <v>156621</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="3">
+        <f t="shared" si="3"/>
+        <v>0.32424392262127005</v>
+      </c>
+      <c r="R6" s="3">
         <f t="shared" si="4"/>
-        <v>495485</v>
-      </c>
-      <c r="R6" s="3">
+        <v>0.35965972733786089</v>
+      </c>
+      <c r="S6" s="3">
         <f t="shared" si="5"/>
-        <v>0.32424392262127005</v>
-      </c>
-      <c r="S6" s="3">
+        <v>0.31609635004086906</v>
+      </c>
+      <c r="T6" s="3">
         <f t="shared" si="6"/>
-        <v>0.35965972733786089</v>
-      </c>
-      <c r="T6" s="3">
-        <f t="shared" si="7"/>
-        <v>0.31609635004086906</v>
-      </c>
-      <c r="U6" s="3">
-        <f t="shared" si="0"/>
         <v>0.14635992871715997</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
@@ -2707,7 +2683,7 @@
         <v>698892</v>
       </c>
       <c r="G7" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>599178</v>
       </c>
       <c r="H7" s="9">
@@ -2717,7 +2693,7 @@
         <v>597150</v>
       </c>
       <c r="J7" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>585051</v>
       </c>
       <c r="K7" s="35">
@@ -2727,7 +2703,7 @@
         <v>698399</v>
       </c>
       <c r="M7" s="31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>547523</v>
       </c>
       <c r="N7" s="4">
@@ -2739,28 +2715,24 @@
       <c r="P7" s="4">
         <v>148484</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="3">
+        <f t="shared" si="3"/>
+        <v>0.31902672722433523</v>
+      </c>
+      <c r="R7" s="3">
         <f t="shared" si="4"/>
-        <v>465892</v>
-      </c>
-      <c r="R7" s="3">
+        <v>0.36226421574098716</v>
+      </c>
+      <c r="S7" s="3">
         <f t="shared" si="5"/>
-        <v>0.31902672722433523</v>
-      </c>
-      <c r="S7" s="3">
+        <v>0.31870905703467756</v>
+      </c>
+      <c r="T7" s="3">
         <f t="shared" si="6"/>
-        <v>0.36226421574098716</v>
-      </c>
-      <c r="T7" s="3">
-        <f t="shared" si="7"/>
-        <v>0.31870905703467756</v>
-      </c>
-      <c r="U7" s="3">
-        <f t="shared" si="0"/>
         <v>0.14479402315811785</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14" t="s">
@@ -2774,25 +2746,24 @@
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
+      <c r="Q8" s="34">
+        <f>AVERAGE(Q2:Q7)</f>
+        <v>0.32429885237709127</v>
+      </c>
       <c r="R8" s="34">
-        <f>AVERAGE(R2:R7)</f>
-        <v>0.32429885237709127</v>
+        <f t="shared" ref="R8:S8" si="7">AVERAGE(R2:R7)</f>
+        <v>0.35655151105876653</v>
       </c>
       <c r="S8" s="34">
-        <f t="shared" ref="S8:T8" si="8">AVERAGE(S2:S7)</f>
-        <v>0.35655151105876653</v>
+        <f t="shared" si="7"/>
+        <v>0.31914963656414214</v>
       </c>
       <c r="T8" s="34">
-        <f t="shared" si="8"/>
-        <v>0.31914963656414214</v>
-      </c>
-      <c r="U8" s="34">
-        <f t="shared" ref="U8" si="9">AVERAGE(U2:U7)</f>
+        <f t="shared" ref="T8" si="8">AVERAGE(T2:T7)</f>
         <v>0.14235112794125368</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
@@ -2811,30 +2782,29 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
+      <c r="Q9" s="13">
+        <f>STDEV(Q2:Q7)</f>
+        <v>6.516576297873982E-3</v>
+      </c>
       <c r="R9" s="13">
-        <f>STDEV(R2:R7)</f>
-        <v>6.516576297873982E-3</v>
+        <f t="shared" ref="R9:S9" si="9">STDEV(R2:R7)</f>
+        <v>8.7321493533673907E-3</v>
       </c>
       <c r="S9" s="13">
-        <f t="shared" ref="S9:T9" si="10">STDEV(S2:S7)</f>
-        <v>8.7321493533673907E-3</v>
+        <f t="shared" si="9"/>
+        <v>3.6029625766548449E-3</v>
       </c>
       <c r="T9" s="13">
-        <f t="shared" si="10"/>
-        <v>3.6029625766548449E-3</v>
-      </c>
-      <c r="U9" s="13">
-        <f t="shared" ref="U9" si="11">STDEV(U2:U7)</f>
+        <f t="shared" ref="T9" si="10">STDEV(T2:T7)</f>
         <v>7.5679150634279475E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
         <v>0</v>
       </c>
@@ -2862,12 +2832,11 @@
       <c r="I13" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="Q13" s="4"/>
+      <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>13</v>
       </c>
@@ -2898,7 +2867,7 @@
         <v>40.101740899841737</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
@@ -2921,15 +2890,15 @@
         <v>38.593000000000004</v>
       </c>
       <c r="H15" s="43">
-        <f t="shared" ref="H15:H19" si="12">E15+F15+G15</f>
+        <f t="shared" ref="H15:H19" si="11">E15+F15+G15</f>
         <v>3432.2719999999999</v>
       </c>
       <c r="I15" s="27">
-        <f t="shared" ref="I15:I19" si="13">(H15/60)/D15*1000000</f>
+        <f t="shared" ref="I15:I19" si="12">(H15/60)/D15*1000000</f>
         <v>46.08467091815087</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
@@ -2952,7 +2921,7 @@
         <v>91.346000000000004</v>
       </c>
       <c r="H16" s="43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>4633.5290000000005</v>
       </c>
       <c r="I16" s="27">
@@ -2983,11 +2952,11 @@
         <v>61.585999999999999</v>
       </c>
       <c r="H17" s="43">
+        <f t="shared" si="11"/>
+        <v>4475.5780000000004</v>
+      </c>
+      <c r="I17" s="27">
         <f t="shared" si="12"/>
-        <v>4475.5780000000004</v>
-      </c>
-      <c r="I17" s="27">
-        <f t="shared" si="13"/>
         <v>53.543973844724107</v>
       </c>
     </row>
@@ -3014,11 +2983,11 @@
         <v>39.314999999999998</v>
       </c>
       <c r="H18" s="43">
+        <f t="shared" si="11"/>
+        <v>3850.9950000000003</v>
+      </c>
+      <c r="I18" s="27">
         <f t="shared" si="12"/>
-        <v>3850.9950000000003</v>
-      </c>
-      <c r="I18" s="27">
-        <f t="shared" si="13"/>
         <v>18.958910753777928</v>
       </c>
     </row>
@@ -3045,11 +3014,11 @@
         <v>106.43600000000001</v>
       </c>
       <c r="H19" s="44">
+        <f t="shared" si="11"/>
+        <v>5227.8039999999992</v>
+      </c>
+      <c r="I19" s="40">
         <f t="shared" si="12"/>
-        <v>5227.8039999999992</v>
-      </c>
-      <c r="I19" s="40">
-        <f t="shared" si="13"/>
         <v>27.079050274960039</v>
       </c>
       <c r="J19" s="27"/>
@@ -3093,11 +3062,837 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE8F7A6-6C4F-B347-A1EA-154638596D00}">
+  <dimension ref="A1:T21"/>
+  <sheetViews>
+    <sheetView zoomScale="111" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="12" width="16.1640625" customWidth="1"/>
+    <col min="13" max="15" width="11.6640625" customWidth="1"/>
+    <col min="16" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2078810</v>
+      </c>
+      <c r="E2" s="42">
+        <v>1191185</v>
+      </c>
+      <c r="F2" s="7">
+        <v>498130</v>
+      </c>
+      <c r="G2" s="30">
+        <f>D2-E2-F2</f>
+        <v>389495</v>
+      </c>
+      <c r="H2">
+        <v>1227784</v>
+      </c>
+      <c r="I2" s="4">
+        <v>477607</v>
+      </c>
+      <c r="J2" s="4">
+        <f>D2-H2-I2</f>
+        <v>373419</v>
+      </c>
+      <c r="K2" s="42">
+        <v>1228922</v>
+      </c>
+      <c r="L2" s="7">
+        <v>497422</v>
+      </c>
+      <c r="M2" s="30">
+        <f>D2-K2-L2</f>
+        <v>352466</v>
+      </c>
+      <c r="N2" s="4">
+        <v>534527</v>
+      </c>
+      <c r="O2" s="4">
+        <v>565310</v>
+      </c>
+      <c r="P2" s="4">
+        <v>554635</v>
+      </c>
+      <c r="Q2" s="3">
+        <f>N2/(N2+O2+P2)</f>
+        <v>0.32308011256763486</v>
+      </c>
+      <c r="R2" s="3">
+        <f>O2/(N2+O2+P2)</f>
+        <v>0.34168604847951489</v>
+      </c>
+      <c r="S2" s="3">
+        <f>P2/(N2+O2+P2)</f>
+        <v>0.33523383895285019</v>
+      </c>
+      <c r="T2" s="3">
+        <f>(N2+O2+P2)/D2</f>
+        <v>0.79587456285086178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1241292</v>
+      </c>
+      <c r="E3" s="32">
+        <v>740747</v>
+      </c>
+      <c r="F3" s="7">
+        <v>267473</v>
+      </c>
+      <c r="G3" s="30">
+        <f t="shared" ref="G3:G7" si="0">D3-E3-F3</f>
+        <v>233072</v>
+      </c>
+      <c r="H3">
+        <v>782782</v>
+      </c>
+      <c r="I3" s="4">
+        <v>232553</v>
+      </c>
+      <c r="J3" s="4">
+        <f t="shared" ref="J3:J7" si="1">D3-H3-I3</f>
+        <v>225957</v>
+      </c>
+      <c r="K3" s="32">
+        <v>762487</v>
+      </c>
+      <c r="L3" s="7">
+        <v>264296</v>
+      </c>
+      <c r="M3" s="30">
+        <f t="shared" ref="M3:M7" si="2">D3-K3-L3</f>
+        <v>214509</v>
+      </c>
+      <c r="N3" s="4">
+        <v>316821</v>
+      </c>
+      <c r="O3" s="4">
+        <v>322205</v>
+      </c>
+      <c r="P3" s="4">
+        <v>332996</v>
+      </c>
+      <c r="Q3" s="3">
+        <f t="shared" ref="Q3:Q7" si="3">N3/(N3+O3+P3)</f>
+        <v>0.32594015361792222</v>
+      </c>
+      <c r="R3" s="3">
+        <f t="shared" ref="R3:R7" si="4">O3/(N3+O3+P3)</f>
+        <v>0.33147912290051046</v>
+      </c>
+      <c r="S3" s="3">
+        <f t="shared" ref="S3:S7" si="5">P3/(N3+O3+P3)</f>
+        <v>0.34258072348156726</v>
+      </c>
+      <c r="T3" s="3">
+        <f t="shared" ref="T3:T7" si="6">(N3+O3+P3)/D3</f>
+        <v>0.78307279834237231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2874064</v>
+      </c>
+      <c r="E4" s="32">
+        <v>1674711</v>
+      </c>
+      <c r="F4" s="7">
+        <v>688541</v>
+      </c>
+      <c r="G4" s="30">
+        <f t="shared" si="0"/>
+        <v>510812</v>
+      </c>
+      <c r="H4">
+        <v>1803367</v>
+      </c>
+      <c r="I4" s="4">
+        <v>573611</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" si="1"/>
+        <v>497086</v>
+      </c>
+      <c r="K4" s="32">
+        <v>1732844</v>
+      </c>
+      <c r="L4" s="7">
+        <v>674657</v>
+      </c>
+      <c r="M4" s="30">
+        <f t="shared" si="2"/>
+        <v>466563</v>
+      </c>
+      <c r="N4" s="4">
+        <v>724676</v>
+      </c>
+      <c r="O4" s="4">
+        <v>716363</v>
+      </c>
+      <c r="P4" s="4">
+        <v>754267</v>
+      </c>
+      <c r="Q4" s="3">
+        <f t="shared" si="3"/>
+        <v>0.33010250051701223</v>
+      </c>
+      <c r="R4" s="3">
+        <f t="shared" si="4"/>
+        <v>0.3263157846787646</v>
+      </c>
+      <c r="S4" s="3">
+        <f t="shared" si="5"/>
+        <v>0.34358171480422317</v>
+      </c>
+      <c r="T4" s="3">
+        <f t="shared" si="6"/>
+        <v>0.76383337323038036</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1393116</v>
+      </c>
+      <c r="E5" s="32">
+        <v>794443</v>
+      </c>
+      <c r="F5" s="7">
+        <v>316903</v>
+      </c>
+      <c r="G5" s="30">
+        <f t="shared" si="0"/>
+        <v>281770</v>
+      </c>
+      <c r="H5">
+        <v>822067</v>
+      </c>
+      <c r="I5" s="4">
+        <v>306821</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" si="1"/>
+        <v>264228</v>
+      </c>
+      <c r="K5" s="32">
+        <v>819859</v>
+      </c>
+      <c r="L5" s="7">
+        <v>319842</v>
+      </c>
+      <c r="M5" s="30">
+        <f t="shared" si="2"/>
+        <v>253415</v>
+      </c>
+      <c r="N5" s="4">
+        <v>363559</v>
+      </c>
+      <c r="O5" s="4">
+        <v>377260</v>
+      </c>
+      <c r="P5" s="4">
+        <v>374745</v>
+      </c>
+      <c r="Q5" s="3">
+        <f t="shared" si="3"/>
+        <v>0.32589703504236422</v>
+      </c>
+      <c r="R5" s="3">
+        <f t="shared" si="4"/>
+        <v>0.33817871498183877</v>
+      </c>
+      <c r="S5" s="3">
+        <f t="shared" si="5"/>
+        <v>0.33592424997579701</v>
+      </c>
+      <c r="T5" s="3">
+        <f t="shared" si="6"/>
+        <v>0.8007689237651423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3385387</v>
+      </c>
+      <c r="E6" s="32">
+        <v>2037031</v>
+      </c>
+      <c r="F6" s="7">
+        <v>697859</v>
+      </c>
+      <c r="G6" s="30">
+        <f t="shared" si="0"/>
+        <v>650497</v>
+      </c>
+      <c r="H6">
+        <v>2135715</v>
+      </c>
+      <c r="I6" s="4">
+        <v>627022</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="1"/>
+        <v>622650</v>
+      </c>
+      <c r="K6" s="32">
+        <v>2094869</v>
+      </c>
+      <c r="L6" s="7">
+        <v>696599</v>
+      </c>
+      <c r="M6" s="30">
+        <f t="shared" si="2"/>
+        <v>593919</v>
+      </c>
+      <c r="N6" s="4">
+        <v>877855</v>
+      </c>
+      <c r="O6" s="4">
+        <v>893333</v>
+      </c>
+      <c r="P6" s="4">
+        <v>910261</v>
+      </c>
+      <c r="Q6" s="3">
+        <f t="shared" si="3"/>
+        <v>0.32738083028989179</v>
+      </c>
+      <c r="R6" s="3">
+        <f t="shared" si="4"/>
+        <v>0.33315308253112402</v>
+      </c>
+      <c r="S6" s="3">
+        <f t="shared" si="5"/>
+        <v>0.33946608717898419</v>
+      </c>
+      <c r="T6" s="3">
+        <f t="shared" si="6"/>
+        <v>0.79206572247131568</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="10">
+        <v>3</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="12">
+        <v>3217619</v>
+      </c>
+      <c r="E7" s="35">
+        <v>1919549</v>
+      </c>
+      <c r="F7" s="12">
+        <v>698892</v>
+      </c>
+      <c r="G7" s="31">
+        <f t="shared" si="0"/>
+        <v>599178</v>
+      </c>
+      <c r="H7" s="9">
+        <v>2035418</v>
+      </c>
+      <c r="I7" s="12">
+        <v>597150</v>
+      </c>
+      <c r="J7" s="12">
+        <f t="shared" si="1"/>
+        <v>585051</v>
+      </c>
+      <c r="K7" s="35">
+        <v>1971697</v>
+      </c>
+      <c r="L7" s="12">
+        <v>698399</v>
+      </c>
+      <c r="M7" s="31">
+        <f t="shared" si="2"/>
+        <v>547523</v>
+      </c>
+      <c r="N7" s="4">
+        <v>806568</v>
+      </c>
+      <c r="O7" s="4">
+        <v>825066</v>
+      </c>
+      <c r="P7" s="4">
+        <v>877265</v>
+      </c>
+      <c r="Q7" s="3">
+        <f t="shared" si="3"/>
+        <v>0.32148284964839158</v>
+      </c>
+      <c r="R7" s="3">
+        <f t="shared" si="4"/>
+        <v>0.32885580487695998</v>
+      </c>
+      <c r="S7" s="3">
+        <f t="shared" si="5"/>
+        <v>0.34966134547464844</v>
+      </c>
+      <c r="T7" s="3">
+        <f t="shared" si="6"/>
+        <v>0.77973775018111213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="32"/>
+      <c r="G8" s="33"/>
+      <c r="K8" s="32"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="34">
+        <f>AVERAGE(Q2:Q7)</f>
+        <v>0.32564724694720276</v>
+      </c>
+      <c r="R8" s="34">
+        <f t="shared" ref="R8:T8" si="7">AVERAGE(R2:R7)</f>
+        <v>0.3332780930747854</v>
+      </c>
+      <c r="S8" s="34">
+        <f t="shared" si="7"/>
+        <v>0.34107465997801167</v>
+      </c>
+      <c r="T8" s="34">
+        <f t="shared" si="7"/>
+        <v>0.78589218847353071</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="13">
+        <f>STDEV(Q2:Q7)</f>
+        <v>3.0638266195295912E-3</v>
+      </c>
+      <c r="R9" s="13">
+        <f t="shared" ref="R9:T9" si="8">STDEV(R2:R7)</f>
+        <v>5.761807035881996E-3</v>
+      </c>
+      <c r="S9" s="13">
+        <f t="shared" si="8"/>
+        <v>5.3947036783344665E-3</v>
+      </c>
+      <c r="T9" s="13">
+        <f t="shared" si="8"/>
+        <v>1.3352864670219556E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2078810</v>
+      </c>
+      <c r="E14" s="32">
+        <v>127.288</v>
+      </c>
+      <c r="F14" s="54">
+        <v>0</v>
+      </c>
+      <c r="G14" s="38">
+        <v>872.63300000000004</v>
+      </c>
+      <c r="H14" s="43">
+        <f>E14+F14+G14</f>
+        <v>999.92100000000005</v>
+      </c>
+      <c r="I14" s="27">
+        <f>(H14/60)/D14*1000000</f>
+        <v>8.0167740197516846</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1241292</v>
+      </c>
+      <c r="E15" s="32">
+        <v>112.88500000000001</v>
+      </c>
+      <c r="F15" s="54">
+        <v>0</v>
+      </c>
+      <c r="G15" s="38">
+        <v>605.16999999999996</v>
+      </c>
+      <c r="H15" s="43">
+        <f t="shared" ref="H15:H19" si="9">E15+F15+G15</f>
+        <v>718.05499999999995</v>
+      </c>
+      <c r="I15" s="27">
+        <f t="shared" ref="I15:I19" si="10">(H15/60)/D15*1000000</f>
+        <v>9.6412313406783667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2874064</v>
+      </c>
+      <c r="E16" s="32">
+        <v>158.345</v>
+      </c>
+      <c r="F16" s="54">
+        <v>0</v>
+      </c>
+      <c r="G16" s="38">
+        <v>1183.47</v>
+      </c>
+      <c r="H16" s="43">
+        <f t="shared" si="9"/>
+        <v>1341.8150000000001</v>
+      </c>
+      <c r="I16" s="27">
+        <f>(H16/60)/D16*1000000</f>
+        <v>7.7811709597744985</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1393116</v>
+      </c>
+      <c r="E17" s="32">
+        <v>119.155</v>
+      </c>
+      <c r="F17" s="54">
+        <v>0</v>
+      </c>
+      <c r="G17" s="38">
+        <v>633.51599999999996</v>
+      </c>
+      <c r="H17" s="43">
+        <f t="shared" si="9"/>
+        <v>752.67099999999994</v>
+      </c>
+      <c r="I17" s="27">
+        <f t="shared" si="10"/>
+        <v>9.0046461792604955</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3385387</v>
+      </c>
+      <c r="E18" s="32">
+        <v>157.904</v>
+      </c>
+      <c r="F18" s="54">
+        <v>0</v>
+      </c>
+      <c r="G18" s="38">
+        <v>1198.7139999999999</v>
+      </c>
+      <c r="H18" s="43">
+        <f t="shared" si="9"/>
+        <v>1356.6179999999999</v>
+      </c>
+      <c r="I18" s="27">
+        <f t="shared" si="10"/>
+        <v>6.6787932960101752</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10">
+        <v>3</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="12">
+        <v>3217619</v>
+      </c>
+      <c r="E19" s="35">
+        <v>158.09700000000001</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0</v>
+      </c>
+      <c r="G19" s="39">
+        <v>1246.165</v>
+      </c>
+      <c r="H19" s="44">
+        <f t="shared" si="9"/>
+        <v>1404.2619999999999</v>
+      </c>
+      <c r="I19" s="40">
+        <f t="shared" si="10"/>
+        <v>7.2738154102976971</v>
+      </c>
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="27">
+        <f>AVERAGE(I14:I19)</f>
+        <v>8.0660718676288212</v>
+      </c>
+      <c r="J20" s="27"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="19"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="40">
+        <f>STDEV(I14:I19)</f>
+        <v>1.0952497467289517</v>
+      </c>
+      <c r="J21" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96560007-93D5-6D4A-BA06-891B98C73FB0}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3114,52 +3909,52 @@
   <sheetData>
     <row r="1" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="49"/>
-      <c r="B1" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50" t="s">
+      <c r="B1" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
     </row>
     <row r="2" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="D2" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="48" t="s">
-        <v>55</v>
-      </c>
       <c r="E2" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="G2" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="48" t="s">
-        <v>55</v>
-      </c>
       <c r="H2" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="J2" s="48" t="s">
         <v>54</v>
-      </c>
-      <c r="J2" s="48" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -3368,7 +4163,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -3376,28 +4171,28 @@
         <v>0</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="51">
+      <c r="B13" s="50">
         <f>C3/(B3+C3+D3)</f>
         <v>0.20674913858639313</v>
       </c>
-      <c r="C13" s="51">
+      <c r="C13" s="50">
         <f>F3/(E3+F3+G3)</f>
         <v>0.21659694776117569</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="50">
         <f>I3/(H3+I3+J3)</f>
         <v>0.20337560680963568</v>
       </c>
@@ -3406,15 +4201,15 @@
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="51">
+      <c r="B14" s="50">
         <f t="shared" ref="B14:B18" si="0">C4/(B4+C4+D4)</f>
         <v>0.20858246489357421</v>
       </c>
-      <c r="C14" s="51">
+      <c r="C14" s="50">
         <f t="shared" ref="C14:C18" si="1">F4/(E4+F4+G4)</f>
         <v>0.22394019907205456</v>
       </c>
-      <c r="D14" s="51">
+      <c r="D14" s="50">
         <f t="shared" ref="D14:D18" si="2">I4/(H4+I4+J4)</f>
         <v>0.21180931310070622</v>
       </c>
@@ -3423,15 +4218,15 @@
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="51">
+      <c r="B15" s="50">
         <f t="shared" si="0"/>
         <v>0.21919290098457439</v>
       </c>
-      <c r="C15" s="51">
+      <c r="C15" s="50">
         <f t="shared" si="1"/>
         <v>0.24112514688069756</v>
       </c>
-      <c r="D15" s="51">
+      <c r="D15" s="50">
         <f t="shared" si="2"/>
         <v>0.22267693258030358</v>
       </c>
@@ -3440,15 +4235,15 @@
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="51">
+      <c r="B16" s="50">
         <f t="shared" si="0"/>
         <v>0.19868273818419066</v>
       </c>
-      <c r="C16" s="51">
+      <c r="C16" s="50">
         <f t="shared" si="1"/>
         <v>0.19990779629515348</v>
       </c>
-      <c r="D16" s="51">
+      <c r="D16" s="50">
         <f t="shared" si="2"/>
         <v>0.19317079220561306</v>
       </c>
@@ -3457,15 +4252,15 @@
       <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="51">
+      <c r="B17" s="50">
         <f t="shared" si="0"/>
         <v>0.20956375207382077</v>
       </c>
-      <c r="C17" s="51">
+      <c r="C17" s="50">
         <f t="shared" si="1"/>
         <v>0.22379966799703316</v>
       </c>
-      <c r="D17" s="51">
+      <c r="D17" s="50">
         <f t="shared" si="2"/>
         <v>0.20710780920514774</v>
       </c>
@@ -3474,51 +4269,51 @@
       <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="52">
+      <c r="B18" s="51">
         <f t="shared" si="0"/>
         <v>0.20870821720506538</v>
       </c>
-      <c r="C18" s="52">
+      <c r="C18" s="51">
         <f t="shared" si="1"/>
         <v>0.22241699802921838</v>
       </c>
-      <c r="D18" s="52">
+      <c r="D18" s="51">
         <f t="shared" si="2"/>
         <v>0.20646549743432641</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="53">
+      <c r="B19" s="52">
         <f>AVERAGE(B13:B18)</f>
         <v>0.2085798686546031</v>
       </c>
-      <c r="C19" s="53">
+      <c r="C19" s="52">
         <f t="shared" ref="C19:D19" si="3">AVERAGE(C13:C18)</f>
         <v>0.22129779267255545</v>
       </c>
-      <c r="D19" s="53">
+      <c r="D19" s="52">
         <f t="shared" si="3"/>
         <v>0.20743432522262215</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
-      <c r="B20" s="54">
+      <c r="B20" s="53">
         <f>STDEV(B13:B18)</f>
         <v>6.5563057592138629E-3</v>
       </c>
-      <c r="C20" s="54">
+      <c r="C20" s="53">
         <f t="shared" ref="C20:D20" si="4">STDEV(C13:C18)</f>
         <v>1.3321022296738129E-2</v>
       </c>
-      <c r="D20" s="54">
+      <c r="D20" s="53">
         <f t="shared" si="4"/>
         <v>9.7205391544923237E-3</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -3526,28 +4321,28 @@
         <v>0</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="51">
+      <c r="B24" s="50">
         <f>C3/(C3+D3)</f>
         <v>0.9039052973486279</v>
       </c>
-      <c r="C24" s="51">
+      <c r="C24" s="50">
         <f>F3/(F3+G3)</f>
         <v>0.88348629368387299</v>
       </c>
-      <c r="D24" s="51">
+      <c r="D24" s="50">
         <f>I3/(I3+J3)</f>
         <v>0.90702835188129305</v>
       </c>
@@ -3556,15 +4351,15 @@
       <c r="A25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="51">
+      <c r="B25" s="50">
         <f t="shared" ref="B25:B29" si="5">C4/(C4+D4)</f>
         <v>0.89371422660506172</v>
       </c>
-      <c r="C25" s="51">
+      <c r="C25" s="50">
         <f t="shared" ref="C25:C29" si="6">F4/(F4+G4)</f>
         <v>0.86537636385926198</v>
       </c>
-      <c r="D25" s="51">
+      <c r="D25" s="50">
         <f t="shared" ref="D25:D29" si="7">I4/(I4+J4)</f>
         <v>0.90014989439258708</v>
       </c>
@@ -3573,15 +4368,15 @@
       <c r="A26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="51">
+      <c r="B26" s="50">
         <f t="shared" si="5"/>
         <v>0.88072525294896176</v>
       </c>
-      <c r="C26" s="51">
+      <c r="C26" s="50">
         <f t="shared" si="6"/>
         <v>0.84557997193632972</v>
       </c>
-      <c r="D26" s="51">
+      <c r="D26" s="50">
         <f t="shared" si="7"/>
         <v>0.89410045176720698</v>
       </c>
@@ -3590,15 +4385,15 @@
       <c r="A27" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="51">
+      <c r="B27" s="50">
         <f t="shared" si="5"/>
         <v>0.89544147843942501</v>
       </c>
-      <c r="C27" s="51">
+      <c r="C27" s="50">
         <f t="shared" si="6"/>
         <v>0.89085526635068024</v>
       </c>
-      <c r="D27" s="51">
+      <c r="D27" s="50">
         <f t="shared" si="7"/>
         <v>0.90331769722814503</v>
       </c>
@@ -3607,15 +4402,15 @@
       <c r="A28" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="51">
+      <c r="B28" s="50">
         <f t="shared" si="5"/>
         <v>0.9010257814736895</v>
       </c>
-      <c r="C28" s="51">
+      <c r="C28" s="50">
         <f t="shared" si="6"/>
         <v>0.88892068729447937</v>
       </c>
-      <c r="D28" s="51">
+      <c r="D28" s="50">
         <f t="shared" si="7"/>
         <v>0.90740066785424689</v>
       </c>
@@ -3624,44 +4419,44 @@
       <c r="A29" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="52">
+      <c r="B29" s="51">
         <f t="shared" si="5"/>
         <v>0.90083562086226387</v>
       </c>
-      <c r="C29" s="52">
+      <c r="C29" s="51">
         <f t="shared" si="6"/>
         <v>0.87129094184007205</v>
       </c>
-      <c r="D29" s="52">
+      <c r="D29" s="51">
         <f t="shared" si="7"/>
         <v>0.90778130977074967</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="53">
+      <c r="B30" s="52">
         <f>AVERAGE(B24:B29)</f>
         <v>0.89594127627967168</v>
       </c>
-      <c r="C30" s="53">
+      <c r="C30" s="52">
         <f t="shared" ref="C30" si="8">AVERAGE(C24:C29)</f>
         <v>0.87425158749411613</v>
       </c>
-      <c r="D30" s="53">
+      <c r="D30" s="52">
         <f t="shared" ref="D30" si="9">AVERAGE(D24:D29)</f>
         <v>0.90329639548237139</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
-      <c r="B31" s="54">
+      <c r="B31" s="53">
         <f>STDEV(B24:B29)</f>
         <v>8.3662338920559316E-3</v>
       </c>
-      <c r="C31" s="54">
+      <c r="C31" s="53">
         <f t="shared" ref="C31:D31" si="10">STDEV(C24:C29)</f>
         <v>1.7237987091810042E-2</v>
       </c>
-      <c r="D31" s="54">
+      <c r="D31" s="53">
         <f t="shared" si="10"/>
         <v>5.3917216197602617E-3</v>
       </c>

</xml_diff>